<commit_message>
changed sample selection because of 3 missing fish
</commit_message>
<xml_diff>
--- a/data/M_menidia_for_bisulfite_size_extremes.xlsx
+++ b/data/M_menidia_for_bisulfite_size_extremes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nt246/github/menidia-selection-experiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7936D0F-8C85-7742-A1A4-2976DE8841D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60254A-5F52-764B-BFC1-1FD38ADFC224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="2320" windowWidth="26840" windowHeight="15940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5380" yWindow="760" windowWidth="26840" windowHeight="15940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ind_included_round1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="129">
   <si>
     <t>SampleID</t>
   </si>
@@ -396,15 +396,9 @@
     <t>round2 (size extremes)</t>
   </si>
   <si>
-    <t>drop</t>
-  </si>
-  <si>
     <t>* Inversion types manually scored based on SNP count in transcriptome data (only variable in D2Gen5)</t>
   </si>
   <si>
-    <t>add? Or do D2Gen5_549 instead for a more average growth?</t>
-  </si>
-  <si>
     <t>U1Gen5_232</t>
   </si>
   <si>
@@ -418,6 +412,18 @@
   </si>
   <si>
     <t>Up2_Gen5</t>
+  </si>
+  <si>
+    <t>considered dropping, but kept</t>
+  </si>
+  <si>
+    <t>added as replacement</t>
+  </si>
+  <si>
+    <t>add? Or do D2Gen5_549 instead for a more average growth? (ended up adding both)</t>
+  </si>
+  <si>
+    <t>sample could not be located, so replaced with 512</t>
   </si>
 </sst>
 </file>
@@ -1844,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -2408,7 +2414,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2708,7 +2714,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2724,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2825,6 +2831,9 @@
         <f>VLOOKUP(A3,Size_extremes!$A$2:$B$41,2,FALSE)</f>
         <v>D2Gen5</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -2916,7 +2925,7 @@
         <v>D2Gen5</v>
       </c>
       <c r="K6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2970,6 +2979,9 @@
       <c r="H8" t="s">
         <v>50</v>
       </c>
+      <c r="K8" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3853,7 +3865,7 @@
         <v>95</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -4016,7 +4028,7 @@
         <v>D2Gen5</v>
       </c>
       <c r="K47" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4148,8 +4160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="A1:B40"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4170,7 +4182,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4178,7 +4190,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4186,7 +4198,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4194,7 +4206,7 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4202,7 +4214,7 @@
         <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4210,7 +4222,7 @@
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4218,7 +4230,7 @@
         <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4226,7 +4238,7 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4234,7 +4246,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4242,7 +4254,7 @@
         <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4250,7 +4262,7 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4258,7 +4270,7 @@
         <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4266,7 +4278,7 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -4274,7 +4286,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -4282,7 +4294,7 @@
         <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4290,7 +4302,7 @@
         <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4298,7 +4310,7 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -4306,7 +4318,7 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -4314,7 +4326,7 @@
         <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -4322,7 +4334,7 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4330,7 +4342,7 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4338,7 +4350,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -4346,7 +4358,7 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -4354,15 +4366,15 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -4370,7 +4382,7 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -4378,7 +4390,7 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4386,7 +4398,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -4394,7 +4406,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -4402,7 +4414,7 @@
         <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4410,7 +4422,7 @@
         <v>23</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4418,7 +4430,7 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -4426,7 +4438,7 @@
         <v>22</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -4434,7 +4446,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -4442,7 +4454,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -4450,7 +4462,7 @@
         <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -4458,7 +4470,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -4466,7 +4478,7 @@
         <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -4474,7 +4486,7 @@
         <v>25</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -4486,8 +4498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987C2DBF-54CF-0342-82D1-9A9B78836033}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4509,7 +4521,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4517,7 +4529,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4525,7 +4537,7 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4533,7 +4545,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4541,7 +4553,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4549,7 +4561,7 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4557,7 +4569,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4565,7 +4577,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4573,7 +4585,7 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4581,7 +4593,7 @@
         <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4589,7 +4601,7 @@
         <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4597,7 +4609,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4605,7 +4617,7 @@
         <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -4613,7 +4625,7 @@
         <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -4621,7 +4633,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4629,7 +4641,7 @@
         <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4637,7 +4649,7 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -4645,7 +4657,7 @@
         <v>88</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -4653,7 +4665,7 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -4661,7 +4673,7 @@
         <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4669,7 +4681,7 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4677,7 +4689,7 @@
         <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -4685,15 +4697,15 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -4701,7 +4713,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -4709,7 +4721,7 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -4717,7 +4729,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4725,7 +4737,7 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -4733,7 +4745,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -4741,7 +4753,7 @@
         <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -4749,7 +4761,7 @@
         <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -4757,7 +4769,7 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -4765,7 +4777,7 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -4773,7 +4785,7 @@
         <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -4781,7 +4793,7 @@
         <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -4789,7 +4801,7 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -4797,7 +4809,7 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -4805,7 +4817,7 @@
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -4813,7 +4825,7 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -4821,7 +4833,7 @@
         <v>24</v>
       </c>
       <c r="B41" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -4829,7 +4841,7 @@
         <v>25</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -4837,7 +4849,7 @@
         <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>